<commit_message>
-Host of changes -Documentation -CPU works with normal memories -Opcode fetch, memory read takes 2 cycles
</commit_message>
<xml_diff>
--- a/docs/Control_Unit_Chart.xlsx
+++ b/docs/Control_Unit_Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soura\Documents\Verilog\BasicCPU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soura\Documents\Verilog\BasicCPU\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51EC689D-7F47-4990-8741-6FD3B08DB852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB02498A-DE7B-49BB-9557-E1534F06CB1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,11 +50,6 @@
     <t>T2</t>
   </si>
   <si>
-    <t>MID &lt;- ir0_mid
-SID &lt;- ir0_sid
-CLR_TIMER &lt;- 1</t>
-  </si>
-  <si>
     <t>AMID &lt;- 1 (AR)
 MID_SID_EN &lt;- 0</t>
   </si>
@@ -126,6 +121,12 @@
     <t>MID &lt;- MEM/ir0_mid
 SID &lt;- ir0_sid
 PC_INR &lt;- 1
+CLR_TIMER &lt;- 1</t>
+  </si>
+  <si>
+    <t>MID &lt;- ir0_mid
+SID &lt;- ir0_sid
+AMID &lt;- 1 (AR) (if mem_wr)
 CLR_TIMER &lt;- 1</t>
   </si>
 </sst>
@@ -266,31 +267,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -305,17 +285,38 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -600,28 +601,29 @@
   <dimension ref="C6:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="4.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="17" width="20.77734375" customWidth="1"/>
+    <col min="5" max="5" width="27.21875" customWidth="1"/>
+    <col min="6" max="17" width="20.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="5"/>
+      <c r="E6" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="15"/>
     </row>
     <row r="7" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C7" s="2" t="s">
@@ -630,154 +632,154 @@
       <c r="D7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="19"/>
+      <c r="G7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="10"/>
+      <c r="K7" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C8" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="15"/>
+      <c r="E8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="10" t="s">
+      <c r="G8" s="3"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="11"/>
-      <c r="K7" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="J8" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="K8" s="9"/>
+      <c r="K8" s="4"/>
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C9" s="14">
+      <c r="C9" s="7">
         <v>1</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="J9" s="11"/>
-      <c r="K9" s="9" t="s">
+      <c r="E9" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="19"/>
+      <c r="G9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" s="10"/>
+      <c r="K9" s="4" t="s">
         <v>3</v>
       </c>
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="3:12" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="15">
+      <c r="C10" s="8">
         <v>2</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="8" t="s">
         <v>4</v>
       </c>
       <c r="E10" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F10" s="17"/>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="H10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="18" t="s">
+      <c r="I10" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="J10" s="19"/>
-      <c r="K10" s="12" t="s">
+      <c r="J10" s="12"/>
+      <c r="K10" s="5" t="s">
         <v>5</v>
       </c>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="3:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C11" s="14">
-        <v>3</v>
-      </c>
-      <c r="D11" s="14" t="s">
+    <row r="11" spans="3:12" ht="72" x14ac:dyDescent="0.3">
+      <c r="C11" s="7">
+        <v>3</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="G11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="3:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C12" s="8">
+        <v>4</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="J11" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="K11" s="9" t="s">
+      <c r="E12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J12" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="L11" s="1"/>
-    </row>
-    <row r="12" spans="3:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C12" s="15">
-        <v>4</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="J12" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="K12" s="9" t="s">
+      <c r="K12" s="4" t="s">
         <v>3</v>
       </c>
       <c r="L12" s="1"/>
@@ -916,6 +918,7 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="C8:D8"/>
     <mergeCell ref="I9:J9"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="I10:J10"/>
@@ -923,7 +926,6 @@
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E7:F7"/>
-    <mergeCell ref="C8:D8"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>